<commit_message>
Second commit with excel formatted
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/Nesto_TestCases.xlsx
+++ b/src/main/resources/testdata/Nesto_TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\EIT PROJECTS\Nesto_Automation_Framework\src\main\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1289EAB7-427A-47E4-932D-C477D0DA6830}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76E633DC-6DB8-40FC-965B-41676E9330F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>TC_ID</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Test Steps</t>
   </si>
@@ -31,31 +28,28 @@
     <t>TC_01</t>
   </si>
   <si>
-    <t>TC_02</t>
-  </si>
-  <si>
-    <t>TC_03</t>
-  </si>
-  <si>
-    <t>Open URL "http://localhost:8080/login"</t>
-  </si>
-  <si>
-    <t>TC_04</t>
-  </si>
-  <si>
-    <t>TC_05</t>
-  </si>
-  <si>
-    <t>Verify that the URL is "http://localhost:8080/dashboard"</t>
-  </si>
-  <si>
-    <t>Click on the "Sign In" button "//button[@type='submit']"</t>
-  </si>
-  <si>
-    <t>Type "shana@gmail.com" into "//input[@placeholder='Enter your email']"</t>
-  </si>
-  <si>
-    <t>Type "shana" into "//input[@placeholder='Enter your password']"</t>
+    <t>Test Case ID(s)</t>
+  </si>
+  <si>
+    <t>Test Case Description</t>
+  </si>
+  <si>
+    <t>1.Open URL "http://localhost:8080/login"</t>
+  </si>
+  <si>
+    <t>2.Type "shana@gmail.com" into "//input[@placeholder='Enter your email']"</t>
+  </si>
+  <si>
+    <t>3.Type "shana" into "//input[@placeholder='Enter your password']"</t>
+  </si>
+  <si>
+    <t>4.Click on the "Sign In" button "//button[@type='submit']"</t>
+  </si>
+  <si>
+    <t>5.Verify that the URL is "http://localhost:8080/dashboard"</t>
+  </si>
+  <si>
+    <t>Testing the Nesto App login page</t>
   </si>
 </sst>
 </file>
@@ -71,12 +65,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -91,8 +91,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -407,59 +408,58 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.44140625" customWidth="1"/>
+    <col min="2" max="2" width="35.44140625" customWidth="1"/>
+    <col min="3" max="3" width="81.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
         <v>6</v>
       </c>
-      <c r="E5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
         <v>7</v>
       </c>
-      <c r="E6" t="s">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Third commit with login page test fixed
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/Nesto_TestCases.xlsx
+++ b/src/main/resources/testdata/Nesto_TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\EIT PROJECTS\Nesto_Automation_Framework\src\main\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76E633DC-6DB8-40FC-965B-41676E9330F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88CB7F78-13A9-4B9F-A514-90B8AC264AD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t>Test Steps</t>
   </si>
@@ -46,10 +46,40 @@
     <t>4.Click on the "Sign In" button "//button[@type='submit']"</t>
   </si>
   <si>
-    <t>5.Verify that the URL is "http://localhost:8080/dashboard"</t>
-  </si>
-  <si>
     <t>Testing the Nesto App login page</t>
+  </si>
+  <si>
+    <t>TC_02</t>
+  </si>
+  <si>
+    <t>Invalid Login Test</t>
+  </si>
+  <si>
+    <t>1. Open URL "http://localhost:8080/login"</t>
+  </si>
+  <si>
+    <t>TC_03</t>
+  </si>
+  <si>
+    <t>Check Signup Link</t>
+  </si>
+  <si>
+    <t>5.Verify that the URL is "dashboard"</t>
+  </si>
+  <si>
+    <t>5.Verify URL is "error"</t>
+  </si>
+  <si>
+    <t>6.Verify text "Invalid Email or Password" at "//div[contains(@class, 'error-msg')]"</t>
+  </si>
+  <si>
+    <t>3.Type "wrongpass123" into "//input[@placeholder='Enter your password']"</t>
+  </si>
+  <si>
+    <t>2.Click on "Register Link" at "//a[@href='/signup']"</t>
+  </si>
+  <si>
+    <t>3.Verify URL is "signup"</t>
   </si>
 </sst>
 </file>
@@ -408,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -437,7 +467,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -460,10 +490,68 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
-        <v>8</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C15" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
seventh commit with signup page test implimented
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/Nesto_TestCases.xlsx
+++ b/src/main/resources/testdata/Nesto_TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\EIT PROJECTS\Nesto_Automation_Framework\src\main\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88CB7F78-13A9-4B9F-A514-90B8AC264AD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{148DDC1D-DC4C-4FE1-83B8-301D463CAF92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
   <si>
     <t>Test Steps</t>
   </si>
@@ -80,6 +80,48 @@
   </si>
   <si>
     <t>3.Verify URL is "signup"</t>
+  </si>
+  <si>
+    <t>TC_04</t>
+  </si>
+  <si>
+    <t>Successful Admin Registration</t>
+  </si>
+  <si>
+    <t>3.Type "newadmin@nesto.com" into "//input[@placeholder='admin@nesto.com']"</t>
+  </si>
+  <si>
+    <t>2.Type "Admin User" into "//input[@placeholder='Enter Full Name']"</t>
+  </si>
+  <si>
+    <t>1.Open URL "http://localhost:8080/signup"</t>
+  </si>
+  <si>
+    <t>4.Type "password123" into "//input[@placeholder='Create Password']"</t>
+  </si>
+  <si>
+    <t>5.Type "30" into "//input[@placeholder='Your Age']"</t>
+  </si>
+  <si>
+    <t>6.Type "9876543210" into "//input[@placeholder='Your Mobile Number']"</t>
+  </si>
+  <si>
+    <t>7.Click on the "Sign Up" button "//button[@type='submit']"</t>
+  </si>
+  <si>
+    <t>8.Verify that the URL is "login"</t>
+  </si>
+  <si>
+    <t>TC_05</t>
+  </si>
+  <si>
+    <t>Navigate back to Login</t>
+  </si>
+  <si>
+    <t>2.Click on "Login here" at "//a[contains(text(), 'Login here')]"</t>
+  </si>
+  <si>
+    <t>3.Verify that the URL is "login"</t>
   </si>
 </sst>
 </file>
@@ -438,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -550,6 +592,73 @@
         <v>19</v>
       </c>
     </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C23" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C26" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Eight commit with signup page test implimented with duplicate mail and mobile number fixed
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/Nesto_TestCases.xlsx
+++ b/src/main/resources/testdata/Nesto_TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\EIT PROJECTS\Nesto_Automation_Framework\src\main\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{148DDC1D-DC4C-4FE1-83B8-301D463CAF92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{587516A8-2D73-46DA-8AB3-D7C221F00004}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -88,9 +88,6 @@
     <t>Successful Admin Registration</t>
   </si>
   <si>
-    <t>3.Type "newadmin@nesto.com" into "//input[@placeholder='admin@nesto.com']"</t>
-  </si>
-  <si>
     <t>2.Type "Admin User" into "//input[@placeholder='Enter Full Name']"</t>
   </si>
   <si>
@@ -103,9 +100,6 @@
     <t>5.Type "30" into "//input[@placeholder='Your Age']"</t>
   </si>
   <si>
-    <t>6.Type "9876543210" into "//input[@placeholder='Your Mobile Number']"</t>
-  </si>
-  <si>
     <t>7.Click on the "Sign Up" button "//button[@type='submit']"</t>
   </si>
   <si>
@@ -122,6 +116,12 @@
   </si>
   <si>
     <t>3.Verify that the URL is "login"</t>
+  </si>
+  <si>
+    <t>3.Type "{RANDOM_EMAIL}" into "//input[@placeholder='admin@nesto.com']"</t>
+  </si>
+  <si>
+    <t>6.Type "{RANDOM_MOBILE}" into "//input[@placeholder='Your Mobile Number']"</t>
   </si>
 </sst>
 </file>
@@ -600,63 +600,63 @@
         <v>21</v>
       </c>
       <c r="C16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C18" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C21" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C22" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C23" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B24" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C25" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C26" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ninth commit with signup and login page test fixed
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/Nesto_TestCases.xlsx
+++ b/src/main/resources/testdata/Nesto_TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\EIT PROJECTS\Nesto_Automation_Framework\src\main\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{587516A8-2D73-46DA-8AB3-D7C221F00004}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D84E46A9-AD21-43FC-9ED5-7A1AEA37A215}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
   <si>
     <t>Test Steps</t>
   </si>
@@ -122,6 +122,33 @@
   </si>
   <si>
     <t>6.Type "{RANDOM_MOBILE}" into "//input[@placeholder='Your Mobile Number']"</t>
+  </si>
+  <si>
+    <t>TC_07</t>
+  </si>
+  <si>
+    <t>Duplicate Email Registration Check</t>
+  </si>
+  <si>
+    <t>2.Type "Duplicate Test" into "//input[@placeholder='Enter Full Name']"</t>
+  </si>
+  <si>
+    <t>3.Type "faizal@nesto.com" into "//input[@placeholder='admin@nesto.com']"</t>
+  </si>
+  <si>
+    <t>4.Type "anyPassword123" into "//input[@placeholder='Create Password']"</t>
+  </si>
+  <si>
+    <t>5.Type "32" into "//input[@placeholder='Your Age']"</t>
+  </si>
+  <si>
+    <t>6.Type "9947110008" into "//input[@placeholder='Your Mobile Number']"</t>
+  </si>
+  <si>
+    <t>9.Verify text "Email already registered. Please login." at "//div[@class='error-alert']"</t>
+  </si>
+  <si>
+    <t>8.Verify URL contains "register"</t>
   </si>
 </sst>
 </file>
@@ -480,10 +507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -659,6 +686,57 @@
         <v>31</v>
       </c>
     </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C28" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C29" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C30" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C31" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C32" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C33" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C34" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="35" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C35" t="s">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Tenth commit with Multi Sheet Runner Implimented
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/Nesto_TestCases.xlsx
+++ b/src/main/resources/testdata/Nesto_TestCases.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\EIT PROJECTS\Nesto_Automation_Framework\src\main\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D84E46A9-AD21-43FC-9ED5-7A1AEA37A215}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4533A20-1FD2-48F7-91EF-980B2F243E97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Auth_Tests" sheetId="1" r:id="rId1"/>
+    <sheet name="Dashboard_Tests" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="49">
   <si>
     <t>Test Steps</t>
   </si>
@@ -124,9 +125,6 @@
     <t>6.Type "{RANDOM_MOBILE}" into "//input[@placeholder='Your Mobile Number']"</t>
   </si>
   <si>
-    <t>TC_07</t>
-  </si>
-  <si>
     <t>Duplicate Email Registration Check</t>
   </si>
   <si>
@@ -149,6 +147,27 @@
   </si>
   <si>
     <t>8.Verify URL contains "register"</t>
+  </si>
+  <si>
+    <t>TC_06</t>
+  </si>
+  <si>
+    <t>TC_DB_01</t>
+  </si>
+  <si>
+    <t>Verify Sidebar Navigation</t>
+  </si>
+  <si>
+    <t>TC_DB_00</t>
+  </si>
+  <si>
+    <t>Prerequisite: Login as Admin</t>
+  </si>
+  <si>
+    <t>1.Click on "Customers" at "//a[contains(@href, '/customers')]"</t>
+  </si>
+  <si>
+    <t>2.Verify URL contains "customers"</t>
   </si>
 </sst>
 </file>
@@ -164,7 +183,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -177,8 +196,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -186,13 +211,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -509,8 +553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -688,10 +732,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27" t="s">
         <v>34</v>
-      </c>
-      <c r="B27" t="s">
-        <v>35</v>
       </c>
       <c r="C27" t="s">
         <v>23</v>
@@ -699,27 +743,27 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C29" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C31" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C32" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.3">
@@ -729,16 +773,97 @@
     </row>
     <row r="34" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C34" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="35" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C35" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00194815-D712-48CB-B57C-1B9F79E9B2F5}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="2" max="2" width="41.88671875" customWidth="1"/>
+    <col min="3" max="3" width="89.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Eleventh commit with Dashboard Testing Partially Implimented
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/Nesto_TestCases.xlsx
+++ b/src/main/resources/testdata/Nesto_TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\EIT PROJECTS\Nesto_Automation_Framework\src\main\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4533A20-1FD2-48F7-91EF-980B2F243E97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E2799CB-A44D-4DDA-88B4-9D7363232BBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="68">
   <si>
     <t>Test Steps</t>
   </si>
@@ -155,9 +155,6 @@
     <t>TC_DB_01</t>
   </si>
   <si>
-    <t>Verify Sidebar Navigation</t>
-  </si>
-  <si>
     <t>TC_DB_00</t>
   </si>
   <si>
@@ -168,6 +165,66 @@
   </si>
   <si>
     <t>2.Verify URL contains "customers"</t>
+  </si>
+  <si>
+    <t>Verify Customers Navigation</t>
+  </si>
+  <si>
+    <t>TC_DB_02</t>
+  </si>
+  <si>
+    <t>Verify Products Navigation</t>
+  </si>
+  <si>
+    <t>1.Click on "Products Link" at "//a[contains(@href, '/products')]"</t>
+  </si>
+  <si>
+    <t>2.Verify URL contains "products"</t>
+  </si>
+  <si>
+    <t>TC_DB_03</t>
+  </si>
+  <si>
+    <t>Verify Sales Navigation</t>
+  </si>
+  <si>
+    <t>1.Click on "Sales Link" at "//a[contains(@href, '/sales')]"</t>
+  </si>
+  <si>
+    <t>2.Verify URL contains "sales"</t>
+  </si>
+  <si>
+    <t>TC_DB_04</t>
+  </si>
+  <si>
+    <t>Verify Dashboard Home Link</t>
+  </si>
+  <si>
+    <t>1.Click on "Dashboard Link" at "//a[contains(@href, '/dashboard')]"</t>
+  </si>
+  <si>
+    <t>2.Verify URL contains "dashboard"</t>
+  </si>
+  <si>
+    <t>TC_DB_05</t>
+  </si>
+  <si>
+    <t>Verify Report Download Button</t>
+  </si>
+  <si>
+    <t>1.Verify text "Download Sales Report" at "//a[contains(@class, 'btn-report')]"</t>
+  </si>
+  <si>
+    <t>TC_DB_06</t>
+  </si>
+  <si>
+    <t>Verify Logout Functionality</t>
+  </si>
+  <si>
+    <t>1.Click on "Logout Button" at "//button[contains(@class, 'btn-logout')]"</t>
+  </si>
+  <si>
+    <t>2.Verify URL contains "login"</t>
   </si>
 </sst>
 </file>
@@ -203,7 +260,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -226,17 +283,71 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -789,10 +900,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00194815-D712-48CB-B57C-1B9F79E9B2F5}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -802,66 +913,261 @@
     <col min="3" max="3" width="89.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="6" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" s="8"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="7" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" s="8"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3" s="8"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4" s="5"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5" s="9"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>43</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
-      <c r="C7" s="3" t="s">
-        <v>48</v>
-      </c>
+      <c r="C7" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Tweleth commit with Pdf Download Test Implimented
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/Nesto_TestCases.xlsx
+++ b/src/main/resources/testdata/Nesto_TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\EIT PROJECTS\Nesto_Automation_Framework\src\main\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E2799CB-A44D-4DDA-88B4-9D7363232BBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{125F8C97-0E5E-491E-A389-55B64CD9CCF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="69">
   <si>
     <t>Test Steps</t>
   </si>
@@ -209,12 +209,6 @@
     <t>TC_DB_05</t>
   </si>
   <si>
-    <t>Verify Report Download Button</t>
-  </si>
-  <si>
-    <t>1.Verify text "Download Sales Report" at "//a[contains(@class, 'btn-report')]"</t>
-  </si>
-  <si>
     <t>TC_DB_06</t>
   </si>
   <si>
@@ -225,6 +219,15 @@
   </si>
   <si>
     <t>2.Verify URL contains "login"</t>
+  </si>
+  <si>
+    <t>Test Sales Report Download</t>
+  </si>
+  <si>
+    <t>1.Click on "Download Button" at "//a[contains(@class, 'btn-report')]"</t>
+  </si>
+  <si>
+    <t>2.Verify "pdf"</t>
   </si>
 </sst>
 </file>
@@ -900,10 +903,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00194815-D712-48CB-B57C-1B9F79E9B2F5}">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1123,11 +1126,11 @@
       <c r="A14" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B14" t="s">
-        <v>62</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>63</v>
+      <c r="B14" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>67</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
@@ -1138,14 +1141,9 @@
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>65</v>
-      </c>
+      <c r="A15" s="5"/>
       <c r="C15" s="5" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
@@ -1156,10 +1154,14 @@
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
+      <c r="A16" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>63</v>
+      </c>
       <c r="C16" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
@@ -1169,6 +1171,20 @@
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
     </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Thirteenth commit with Database connection and dashboard test Implimented
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/Nesto_TestCases.xlsx
+++ b/src/main/resources/testdata/Nesto_TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\EIT PROJECTS\Nesto_Automation_Framework\src\main\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{125F8C97-0E5E-491E-A389-55B64CD9CCF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9696EE72-BA25-4ABF-BAA1-C4DCE37EDF65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="78">
   <si>
     <t>Test Steps</t>
   </si>
@@ -228,6 +228,33 @@
   </si>
   <si>
     <t>2.Verify "pdf"</t>
+  </si>
+  <si>
+    <t>Verify Live Customer Count</t>
+  </si>
+  <si>
+    <t>TC_DB_08</t>
+  </si>
+  <si>
+    <t>1.Verify text "{DB_QUERY}SELECT COUNT(*) FROM customers" at "//h5[text()='Total Customers']/following-sibling::h2"</t>
+  </si>
+  <si>
+    <t>TC_DB_07</t>
+  </si>
+  <si>
+    <t>Verify Live Product Count</t>
+  </si>
+  <si>
+    <t>1.Verify text "{DB_QUERY}SELECT COUNT(*) FROM products" at "//h5[text()='Total Products']/following-sibling::h2"</t>
+  </si>
+  <si>
+    <t>Verify Live Revenue</t>
+  </si>
+  <si>
+    <t>1.Verify text "{DB_QUERY}SELECT SUM(total_bill) FROM sales" at "//h5[text()='Total Revenue']/following-sibling::h2"</t>
+  </si>
+  <si>
+    <t>TC_DB_09</t>
   </si>
 </sst>
 </file>
@@ -903,17 +930,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00194815-D712-48CB-B57C-1B9F79E9B2F5}">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="41.88671875" customWidth="1"/>
-    <col min="3" max="3" width="89.6640625" customWidth="1"/>
+    <col min="3" max="3" width="107.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
@@ -1126,7 +1153,7 @@
       <c r="A14" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="11" t="s">
         <v>66</v>
       </c>
       <c r="C14" s="3" t="s">
@@ -1142,7 +1169,8 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
-      <c r="C15" s="5" t="s">
+      <c r="B15" s="5"/>
+      <c r="C15" s="3" t="s">
         <v>68</v>
       </c>
       <c r="D15" s="5"/>
@@ -1158,10 +1186,10 @@
         <v>62</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>64</v>
+        <v>69</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
@@ -1172,10 +1200,14 @@
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5" t="s">
-        <v>65</v>
+      <c r="A17" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C17" t="s">
+        <v>74</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
@@ -1185,6 +1217,92 @@
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
     </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fifteenth commit with Customer Page test started
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/Nesto_TestCases.xlsx
+++ b/src/main/resources/testdata/Nesto_TestCases.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\EIT PROJECTS\Nesto_Automation_Framework\src\main\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9696EE72-BA25-4ABF-BAA1-C4DCE37EDF65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CEA2BB0-E7D9-413A-970B-87978818DBD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Auth_Tests" sheetId="1" r:id="rId1"/>
     <sheet name="Dashboard_Tests" sheetId="2" r:id="rId2"/>
+    <sheet name="Customer_Tests" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="79">
   <si>
     <t>Test Steps</t>
   </si>
@@ -212,15 +213,6 @@
     <t>TC_DB_06</t>
   </si>
   <si>
-    <t>Verify Logout Functionality</t>
-  </si>
-  <si>
-    <t>1.Click on "Logout Button" at "//button[contains(@class, 'btn-logout')]"</t>
-  </si>
-  <si>
-    <t>2.Verify URL contains "login"</t>
-  </si>
-  <si>
     <t>Test Sales Report Download</t>
   </si>
   <si>
@@ -254,7 +246,19 @@
     <t>1.Verify text "{DB_QUERY}SELECT SUM(total_bill) FROM sales" at "//h5[text()='Total Revenue']/following-sibling::h2"</t>
   </si>
   <si>
-    <t>TC_DB_09</t>
+    <t>TC_CUST_01</t>
+  </si>
+  <si>
+    <t>Navigate to Customers</t>
+  </si>
+  <si>
+    <t>TC_CUST_02</t>
+  </si>
+  <si>
+    <t>Verify List Consistency</t>
+  </si>
+  <si>
+    <t>1.Verify text "{DB_QUERY}SELECT COUNT(*) FROM customers" at "//table/tbody/tr"</t>
   </si>
 </sst>
 </file>
@@ -932,8 +936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00194815-D712-48CB-B57C-1B9F79E9B2F5}">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1154,10 +1158,10 @@
         <v>61</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
@@ -1171,7 +1175,7 @@
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
@@ -1186,10 +1190,10 @@
         <v>62</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
@@ -1201,13 +1205,13 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C17" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
@@ -1219,13 +1223,13 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
@@ -1236,15 +1240,9 @@
       <c r="J18" s="5"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>64</v>
-      </c>
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="3"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
@@ -1256,9 +1254,7 @@
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
-      <c r="C20" s="3" t="s">
-        <v>65</v>
-      </c>
+      <c r="C20" s="3"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
@@ -1306,4 +1302,62 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A3A8CE0-7C44-4B95-881A-8E4CBACAD140}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.5546875" customWidth="1"/>
+    <col min="2" max="2" width="53.21875" customWidth="1"/>
+    <col min="3" max="3" width="97.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
sixteenth commit with add customer fixed
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/Nesto_TestCases.xlsx
+++ b/src/main/resources/testdata/Nesto_TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\EIT PROJECTS\Nesto_Automation_Framework\src\main\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CEA2BB0-E7D9-413A-970B-87978818DBD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D822740D-47CB-4160-8829-D8D0883E2708}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="91">
   <si>
     <t>Test Steps</t>
   </si>
@@ -259,6 +259,42 @@
   </si>
   <si>
     <t>1.Verify text "{DB_QUERY}SELECT COUNT(*) FROM customers" at "//table/tbody/tr"</t>
+  </si>
+  <si>
+    <t>TC_CUST_03</t>
+  </si>
+  <si>
+    <t>Add New Customer</t>
+  </si>
+  <si>
+    <t>2.Click on "Add New Customer" at "//a[contains(@class, 'btn-add')]"</t>
+  </si>
+  <si>
+    <t>3.Type "Automation User" at "//input[@name='name']"</t>
+  </si>
+  <si>
+    <t>4.Type "auto@nesto.com" at "//input[@name='email']"</t>
+  </si>
+  <si>
+    <t>5.Type "9876543210" at "//input[@name='mobile']"</t>
+  </si>
+  <si>
+    <t>6.Click on "//button[@type='submit']"</t>
+  </si>
+  <si>
+    <t>TC_CUST_04</t>
+  </si>
+  <si>
+    <t>Verify Entry</t>
+  </si>
+  <si>
+    <t>1.dbexecute "{DB_QUERY}DELETE FROM customers WHERE email='auto@nesto.com'" at ""</t>
+  </si>
+  <si>
+    <t>1.Open URL "http://localhost:8080/customers"</t>
+  </si>
+  <si>
+    <t>2.Verify text "{DB_QUERY}SELECT name FROM customers WHERE email='auto@nesto.com'" at "//tr[td[contains(text(),'auto@nesto.com')]]/td[2]"</t>
   </si>
 </sst>
 </file>
@@ -1306,17 +1342,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A3A8CE0-7C44-4B95-881A-8E4CBACAD140}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25.5546875" customWidth="1"/>
-    <col min="2" max="2" width="53.21875" customWidth="1"/>
-    <col min="3" max="3" width="97.5546875" customWidth="1"/>
+    <col min="2" max="2" width="25.33203125" customWidth="1"/>
+    <col min="3" max="3" width="128" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -1357,6 +1393,58 @@
         <v>78</v>
       </c>
     </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>86</v>
+      </c>
+      <c r="B11" t="s">
+        <v>87</v>
+      </c>
+      <c r="C11" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
+        <v>90</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
sevententh commit with pdf bug fixed
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/Nesto_TestCases.xlsx
+++ b/src/main/resources/testdata/Nesto_TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\EIT PROJECTS\Nesto_Automation_Framework\src\main\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D822740D-47CB-4160-8829-D8D0883E2708}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF4D463C-3D8A-4370-917C-70A57D3D6175}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Auth_Tests" sheetId="1" r:id="rId1"/>
@@ -219,9 +219,6 @@
     <t>1.Click on "Download Button" at "//a[contains(@class, 'btn-report')]"</t>
   </si>
   <si>
-    <t>2.Verify "pdf"</t>
-  </si>
-  <si>
     <t>Verify Live Customer Count</t>
   </si>
   <si>
@@ -295,6 +292,9 @@
   </si>
   <si>
     <t>2.Verify text "{DB_QUERY}SELECT name FROM customers WHERE email='auto@nesto.com'" at "//tr[td[contains(text(),'auto@nesto.com')]]/td[2]"</t>
+  </si>
+  <si>
+    <t>2.Verify ".pdf"</t>
   </si>
 </sst>
 </file>
@@ -972,8 +972,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00194815-D712-48CB-B57C-1B9F79E9B2F5}">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1211,7 +1211,7 @@
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="3" t="s">
-        <v>65</v>
+        <v>90</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
@@ -1226,10 +1226,10 @@
         <v>62</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
@@ -1241,13 +1241,13 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="C17" t="s">
         <v>70</v>
-      </c>
-      <c r="C17" t="s">
-        <v>71</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
@@ -1259,13 +1259,13 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B18" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>72</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>73</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
@@ -1344,7 +1344,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A3A8CE0-7C44-4B95-881A-8E4CBACAD140}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -1368,10 +1368,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" t="s">
         <v>74</v>
-      </c>
-      <c r="B2" t="s">
-        <v>75</v>
       </c>
       <c r="C2" t="s">
         <v>46</v>
@@ -1384,65 +1384,65 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" t="s">
         <v>76</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>77</v>
-      </c>
-      <c r="C4" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" t="s">
         <v>79</v>
       </c>
-      <c r="B5" t="s">
-        <v>80</v>
-      </c>
       <c r="C5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>85</v>
+      </c>
+      <c r="B11" t="s">
         <v>86</v>
       </c>
-      <c r="B11" t="s">
-        <v>87</v>
-      </c>
       <c r="C11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
eigtheenth commit with customer side test completed
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/Nesto_TestCases.xlsx
+++ b/src/main/resources/testdata/Nesto_TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\EIT PROJECTS\Nesto_Automation_Framework\src\main\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF4D463C-3D8A-4370-917C-70A57D3D6175}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87D05B7E-3C73-40AD-AFBF-0449A8EED563}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Auth_Tests" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="101">
   <si>
     <t>Test Steps</t>
   </si>
@@ -295,6 +295,36 @@
   </si>
   <si>
     <t>2.Verify ".pdf"</t>
+  </si>
+  <si>
+    <t>TC_CUST_05</t>
+  </si>
+  <si>
+    <t>Edit Customer Details</t>
+  </si>
+  <si>
+    <t>1.Click "Edit Button" at "//tr[td[text()='auto@nesto.com']]//a[contains(@class, 'btn-outline-primary')]"</t>
+  </si>
+  <si>
+    <t>2.Type "Automation User Updated" at "//input[@name='name']"</t>
+  </si>
+  <si>
+    <t>3.Click "Save Customer" at "//button[contains(@class, 'btn-save')]"</t>
+  </si>
+  <si>
+    <t>4.Verify text "{DB_QUERY}SELECT name FROM customers WHERE email='auto@nesto.com'" at "//tr[td[text()='auto@nesto.com']]/td[2]"</t>
+  </si>
+  <si>
+    <t>TC_CUST_06</t>
+  </si>
+  <si>
+    <t>Delete Customer</t>
+  </si>
+  <si>
+    <t>1.Click "Delete Button" at "//tr[td[text()='auto@nesto.com']]//a[contains(@class, 'btn-outline-danger')]"</t>
+  </si>
+  <si>
+    <t>2.Verify text "{DB_QUERY}SELECT COUNT(*) FROM customers WHERE email='auto@nesto.com'" at "//table/tbody/tr[td[text()='auto@nesto.com']]"</t>
   </si>
 </sst>
 </file>
@@ -972,7 +1002,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00194815-D712-48CB-B57C-1B9F79E9B2F5}">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -1342,10 +1372,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A3A8CE0-7C44-4B95-881A-8E4CBACAD140}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1445,6 +1475,48 @@
         <v>89</v>
       </c>
     </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>91</v>
+      </c>
+      <c r="B13" t="s">
+        <v>92</v>
+      </c>
+      <c r="C13" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C14" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C15" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C16" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>97</v>
+      </c>
+      <c r="B17" t="s">
+        <v>98</v>
+      </c>
+      <c r="C17" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C18" t="s">
+        <v>100</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
ninteenth commit with product side test started
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/Nesto_TestCases.xlsx
+++ b/src/main/resources/testdata/Nesto_TestCases.xlsx
@@ -8,21 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\EIT PROJECTS\Nesto_Automation_Framework\src\main\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87D05B7E-3C73-40AD-AFBF-0449A8EED563}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C990884-2B1C-499F-ADC3-144CF4D54886}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Auth_Tests" sheetId="1" r:id="rId1"/>
     <sheet name="Dashboard_Tests" sheetId="2" r:id="rId2"/>
     <sheet name="Customer_Tests" sheetId="3" r:id="rId3"/>
+    <sheet name="Product_Tests" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="105">
   <si>
     <t>Test Steps</t>
   </si>
@@ -325,6 +326,18 @@
   </si>
   <si>
     <t>2.Verify text "{DB_QUERY}SELECT COUNT(*) FROM customers WHERE email='auto@nesto.com'" at "//table/tbody/tr[td[text()='auto@nesto.com']]"</t>
+  </si>
+  <si>
+    <t>TC_PROD_01</t>
+  </si>
+  <si>
+    <t>Navigate to Products</t>
+  </si>
+  <si>
+    <t>1.Click on "Products" at "//a[contains(@href, '/products')]"</t>
+  </si>
+  <si>
+    <t>2 Verify URL contains "products"</t>
   </si>
 </sst>
 </file>
@@ -771,8 +784,8 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.44140625" customWidth="1"/>
-    <col min="2" max="2" width="35.44140625" customWidth="1"/>
-    <col min="3" max="3" width="81.6640625" customWidth="1"/>
+    <col min="2" max="2" width="32" customWidth="1"/>
+    <col min="3" max="3" width="74.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -1009,8 +1022,8 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="41.88671875" customWidth="1"/>
-    <col min="3" max="3" width="107.5546875" customWidth="1"/>
+    <col min="2" max="2" width="31.77734375" customWidth="1"/>
+    <col min="3" max="3" width="99.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
@@ -1374,15 +1387,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A3A8CE0-7C44-4B95-881A-8E4CBACAD140}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.5546875" customWidth="1"/>
-    <col min="2" max="2" width="25.33203125" customWidth="1"/>
-    <col min="3" max="3" width="128" customWidth="1"/>
+    <col min="1" max="1" width="15.77734375" customWidth="1"/>
+    <col min="2" max="2" width="22.21875" customWidth="1"/>
+    <col min="3" max="3" width="124.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -1520,4 +1533,51 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58BDEBBA-0125-41E5-9F1F-7F05B5F47116}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.88671875" customWidth="1"/>
+    <col min="2" max="2" width="40.5546875" customWidth="1"/>
+    <col min="3" max="3" width="106.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
twententh commit with add product completed
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/Nesto_TestCases.xlsx
+++ b/src/main/resources/testdata/Nesto_TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\EIT PROJECTS\Nesto_Automation_Framework\src\main\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C990884-2B1C-499F-ADC3-144CF4D54886}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2339937-48F7-46E2-A52E-33502CD7E898}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="118">
   <si>
     <t>Test Steps</t>
   </si>
@@ -338,6 +338,45 @@
   </si>
   <si>
     <t>2 Verify URL contains "products"</t>
+  </si>
+  <si>
+    <t>TC_PROD_02</t>
+  </si>
+  <si>
+    <t>1. Verify text "{DB_QUERY}SELECT COUNT(*) FROM products" at "//table/tbody/tr"</t>
+  </si>
+  <si>
+    <t>TC_PROD_03</t>
+  </si>
+  <si>
+    <t>Add New Product</t>
+  </si>
+  <si>
+    <t>1.dbexecute "{DB_QUERY}DELETE FROM products WHERE name='Auto Product'" at ""</t>
+  </si>
+  <si>
+    <t>2.Click on "Add New Product" at "//a[contains(@class, 'btn-add')]"</t>
+  </si>
+  <si>
+    <t>3.Type "Auto Product" at "//input[@name='name']"</t>
+  </si>
+  <si>
+    <t>4.Type "499.00" at "//input[@name='price']"</t>
+  </si>
+  <si>
+    <t>5.Type "2026-12-31" at "//input[@name='expiryDate']"</t>
+  </si>
+  <si>
+    <t>TC_PROD_04</t>
+  </si>
+  <si>
+    <t>Verify Product Entry</t>
+  </si>
+  <si>
+    <t>1.Open URL "http://localhost:8080/products"</t>
+  </si>
+  <si>
+    <t>2.Verify text "{DB_QUERY}SELECT name FROM products WHERE name='Auto Product'" at "//tr[td[text()='Auto Product']]/td[2]"</t>
   </si>
 </sst>
 </file>
@@ -1537,17 +1576,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58BDEBBA-0125-41E5-9F1F-7F05B5F47116}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.88671875" customWidth="1"/>
     <col min="2" max="2" width="40.5546875" customWidth="1"/>
-    <col min="3" max="3" width="106.5546875" customWidth="1"/>
+    <col min="3" max="3" width="102.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -1577,6 +1616,69 @@
         <v>104</v>
       </c>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C7" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>114</v>
+      </c>
+      <c r="B11" t="s">
+        <v>115</v>
+      </c>
+      <c r="C11" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
+        <v>117</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
twentyoneth commit with product testing completed
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/Nesto_TestCases.xlsx
+++ b/src/main/resources/testdata/Nesto_TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\EIT PROJECTS\Nesto_Automation_Framework\src\main\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2339937-48F7-46E2-A52E-33502CD7E898}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E33F2CB-5650-4603-96EA-CA0771844F5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="129">
   <si>
     <t>Test Steps</t>
   </si>
@@ -352,9 +352,6 @@
     <t>Add New Product</t>
   </si>
   <si>
-    <t>1.dbexecute "{DB_QUERY}DELETE FROM products WHERE name='Auto Product'" at ""</t>
-  </si>
-  <si>
     <t>2.Click on "Add New Product" at "//a[contains(@class, 'btn-add')]"</t>
   </si>
   <si>
@@ -377,6 +374,42 @@
   </si>
   <si>
     <t>2.Verify text "{DB_QUERY}SELECT name FROM products WHERE name='Auto Product'" at "//tr[td[text()='Auto Product']]/td[2]"</t>
+  </si>
+  <si>
+    <t>TC_PROD_05</t>
+  </si>
+  <si>
+    <t>1.Click "Edit Button" at "//tr[td[text()='Auto Product']]//a[contains(@class, 'btn-outline-primary')]"</t>
+  </si>
+  <si>
+    <t>Edit Product Details</t>
+  </si>
+  <si>
+    <t>2.Type "Auto Product Updated" at "//input[@name='name']"</t>
+  </si>
+  <si>
+    <t>3.Type "2026-12-31" at "//input[@name='expiryDate']"</t>
+  </si>
+  <si>
+    <t>4.Click "Save Product" at "//button[@type='submit']" (Fixed @ symbol)</t>
+  </si>
+  <si>
+    <t>5.Verify text "{DB_QUERY}SELECT name FROM products WHERE name='Auto Product Updated'" at "//tr[td[text()='Auto Product Updated']]/td[2]"</t>
+  </si>
+  <si>
+    <t>1.dbexecute "{DB_QUERY}DELETE FROM products WHERE TRIM(name) = 'Auto Product'" at ""</t>
+  </si>
+  <si>
+    <t>TC_PROD_06</t>
+  </si>
+  <si>
+    <t>Delete Product</t>
+  </si>
+  <si>
+    <t>1.Click "Delete Button" at "//tr[td[text()='Auto Product Updated']]//a[contains(@class, 'btn-outline-danger')]"</t>
+  </si>
+  <si>
+    <t>2.Verify text "{DB_QUERY}SELECT COUNT(*) FROM products WHERE name='Auto Product Updated'" at "//tr[td[text()='Auto Product Updated']]"</t>
   </si>
 </sst>
 </file>
@@ -1427,7 +1460,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1576,17 +1609,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58BDEBBA-0125-41E5-9F1F-7F05B5F47116}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.88671875" customWidth="1"/>
-    <col min="2" max="2" width="40.5546875" customWidth="1"/>
-    <col min="3" max="3" width="102.33203125" customWidth="1"/>
+    <col min="1" max="1" width="14.5546875" customWidth="1"/>
+    <col min="2" max="2" width="27" customWidth="1"/>
+    <col min="3" max="3" width="121.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -1635,27 +1668,27 @@
         <v>108</v>
       </c>
       <c r="C5" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -1665,18 +1698,65 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>113</v>
+      </c>
+      <c r="B11" t="s">
         <v>114</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>115</v>
-      </c>
-      <c r="C11" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C12" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>117</v>
+      </c>
+      <c r="B13" t="s">
+        <v>119</v>
+      </c>
+      <c r="C13" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C14" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C15" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C16" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C17" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>125</v>
+      </c>
+      <c r="B18" t="s">
+        <v>126</v>
+      </c>
+      <c r="C18" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C19" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
twentysecondth commit with sales testing started
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/Nesto_TestCases.xlsx
+++ b/src/main/resources/testdata/Nesto_TestCases.xlsx
@@ -8,22 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\EIT PROJECTS\Nesto_Automation_Framework\src\main\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E33F2CB-5650-4603-96EA-CA0771844F5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3671A3EE-1AC3-495D-8E58-F9D3F891B259}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Auth_Tests" sheetId="1" r:id="rId1"/>
     <sheet name="Dashboard_Tests" sheetId="2" r:id="rId2"/>
     <sheet name="Customer_Tests" sheetId="3" r:id="rId3"/>
     <sheet name="Product_Tests" sheetId="4" r:id="rId4"/>
+    <sheet name="Sales_Tests" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="131">
   <si>
     <t>Test Steps</t>
   </si>
@@ -337,9 +338,6 @@
     <t>1.Click on "Products" at "//a[contains(@href, '/products')]"</t>
   </si>
   <si>
-    <t>2 Verify URL contains "products"</t>
-  </si>
-  <si>
     <t>TC_PROD_02</t>
   </si>
   <si>
@@ -410,6 +408,15 @@
   </si>
   <si>
     <t>2.Verify text "{DB_QUERY}SELECT COUNT(*) FROM products WHERE name='Auto Product Updated'" at "//tr[td[text()='Auto Product Updated']]"</t>
+  </si>
+  <si>
+    <t>TC_SALE_01</t>
+  </si>
+  <si>
+    <t>Navigate to Sales</t>
+  </si>
+  <si>
+    <t>1.Click on "Sales" at "//a[contains(@href, '/sales')]"</t>
   </si>
 </sst>
 </file>
@@ -1611,14 +1618,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58BDEBBA-0125-41E5-9F1F-7F05B5F47116}">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.5546875" customWidth="1"/>
-    <col min="2" max="2" width="27" customWidth="1"/>
+    <col min="2" max="2" width="23.109375" customWidth="1"/>
     <col min="3" max="3" width="121.44140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1646,49 +1653,49 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
-        <v>104</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B4" t="s">
         <v>76</v>
       </c>
       <c r="C4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B5" t="s">
         <v>107</v>
       </c>
-      <c r="B5" t="s">
-        <v>108</v>
-      </c>
       <c r="C5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -1698,65 +1705,112 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>112</v>
+      </c>
+      <c r="B11" t="s">
         <v>113</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>114</v>
-      </c>
-      <c r="C11" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>116</v>
+      </c>
+      <c r="B13" t="s">
+        <v>118</v>
+      </c>
+      <c r="C13" t="s">
         <v>117</v>
-      </c>
-      <c r="B13" t="s">
-        <v>119</v>
-      </c>
-      <c r="C13" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C17" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>124</v>
+      </c>
+      <c r="B18" t="s">
         <v>125</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>126</v>
-      </c>
-      <c r="C18" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C19" t="s">
+        <v>127</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA48A5FA-3EC7-484B-B419-BAAFFEFDA622}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.21875" customWidth="1"/>
+    <col min="2" max="2" width="28.6640625" customWidth="1"/>
+    <col min="3" max="3" width="114.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>128</v>
+      </c>
+      <c r="B2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
23rd commit with sales list verified
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/Nesto_TestCases.xlsx
+++ b/src/main/resources/testdata/Nesto_TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\EIT PROJECTS\Nesto_Automation_Framework\src\main\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3671A3EE-1AC3-495D-8E58-F9D3F891B259}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E194489-E6C2-493D-AC88-AC25567B186F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="133">
   <si>
     <t>Test Steps</t>
   </si>
@@ -417,6 +417,12 @@
   </si>
   <si>
     <t>1.Click on "Sales" at "//a[contains(@href, '/sales')]"</t>
+  </si>
+  <si>
+    <t>TC_SALE_02</t>
+  </si>
+  <si>
+    <t>1.Verify text "{DB_QUERY}SELECT COUNT(*) FROM sales" at "//table/tbody/tr"</t>
   </si>
 </sst>
 </file>
@@ -1619,7 +1625,7 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1773,10 +1779,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA48A5FA-3EC7-484B-B419-BAAFFEFDA622}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1813,6 +1819,17 @@
         <v>56</v>
       </c>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" t="s">
+        <v>132</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
24th commit with create sale fixed
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/Nesto_TestCases.xlsx
+++ b/src/main/resources/testdata/Nesto_TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\EIT PROJECTS\Nesto_Automation_Framework\src\main\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E194489-E6C2-493D-AC88-AC25567B186F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF664637-1996-4678-9ECF-1D67568D9F60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="146">
   <si>
     <t>Test Steps</t>
   </si>
@@ -423,6 +423,45 @@
   </si>
   <si>
     <t>1.Verify text "{DB_QUERY}SELECT COUNT(*) FROM sales" at "//table/tbody/tr"</t>
+  </si>
+  <si>
+    <t>TC_SALE_03</t>
+  </si>
+  <si>
+    <t>Create Multi-Item Sale</t>
+  </si>
+  <si>
+    <t>TC_SALE_04</t>
+  </si>
+  <si>
+    <t>Verify Invoice &amp; Print</t>
+  </si>
+  <si>
+    <t>1.Verify URL contains "invoice"</t>
+  </si>
+  <si>
+    <t>1.Click "Create New Sale" at "//a[contains(@class, 'btn-create')]"</t>
+  </si>
+  <si>
+    <t>2.Type "faizal" at "//select[@name='customerId']"</t>
+  </si>
+  <si>
+    <t>3.Type "Dettol (₹80.0)" at "(//select[@name='productIds'])[1]"</t>
+  </si>
+  <si>
+    <t>4.Type "3" at "(//input[@name='quantities'])[1]"</t>
+  </si>
+  <si>
+    <t>5.Click "Add Item" at "//button[contains(text(), '+ Add Another Item')]"</t>
+  </si>
+  <si>
+    <t>6.Type "Pears Soap (₹40.0)" at "(//select[@name='productIds'])[2]"</t>
+  </si>
+  <si>
+    <t>7.Type "2" at "(//input[@name='quantities'])[2]"</t>
+  </si>
+  <si>
+    <t>8.Click "Generate Bill" at "//button[@type='submit']"</t>
   </si>
 </sst>
 </file>
@@ -1779,10 +1818,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA48A5FA-3EC7-484B-B419-BAAFFEFDA622}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1830,6 +1869,63 @@
         <v>132</v>
       </c>
     </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B5" t="s">
+        <v>134</v>
+      </c>
+      <c r="C5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C7" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C11" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>135</v>
+      </c>
+      <c r="B13" t="s">
+        <v>136</v>
+      </c>
+      <c r="C13" t="s">
+        <v>137</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
25th commit with invoice verified
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/Nesto_TestCases.xlsx
+++ b/src/main/resources/testdata/Nesto_TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\EIT PROJECTS\Nesto_Automation_Framework\src\main\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF664637-1996-4678-9ECF-1D67568D9F60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF4E30C2-B9DB-4B06-911E-0A10D33586AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="150">
   <si>
     <t>Test Steps</t>
   </si>
@@ -462,6 +462,18 @@
   </si>
   <si>
     <t>8.Click "Generate Bill" at "//button[@type='submit']"</t>
+  </si>
+  <si>
+    <t>2.Verify text "faizal" at "//strong[text()='Customer:']/following-sibling::span"</t>
+  </si>
+  <si>
+    <t>3.Verify text "Dettol" at "//table/tbody/tr[1]/td[1]"</t>
+  </si>
+  <si>
+    <t>4.Verify text "Pears Soap" at "//table/tbody/tr[2]/td[1]"</t>
+  </si>
+  <si>
+    <t>5.Click "Back" at "//a[text()='Back']"</t>
   </si>
 </sst>
 </file>
@@ -1818,10 +1830,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA48A5FA-3EC7-484B-B419-BAAFFEFDA622}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1926,6 +1938,26 @@
         <v>137</v>
       </c>
     </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C15" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C16" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C17" t="s">
+        <v>149</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
26th commit with sales and logout completed
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/Nesto_TestCases.xlsx
+++ b/src/main/resources/testdata/Nesto_TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\EIT PROJECTS\Nesto_Automation_Framework\src\main\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF4E30C2-B9DB-4B06-911E-0A10D33586AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C185C60D-8527-484E-9F78-A2783830AAF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Auth_Tests" sheetId="1" r:id="rId1"/>
@@ -18,13 +18,14 @@
     <sheet name="Customer_Tests" sheetId="3" r:id="rId3"/>
     <sheet name="Product_Tests" sheetId="4" r:id="rId4"/>
     <sheet name="Sales_Tests" sheetId="5" r:id="rId5"/>
+    <sheet name="Logout_Tests" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="158">
   <si>
     <t>Test Steps</t>
   </si>
@@ -474,6 +475,30 @@
   </si>
   <si>
     <t>5.Click "Back" at "//a[text()='Back']"</t>
+  </si>
+  <si>
+    <t>Verify List Consistency &amp; Invoice</t>
+  </si>
+  <si>
+    <t>3.Verify URL contains "invoice"</t>
+  </si>
+  <si>
+    <t>4.Verify text "NESTO SUPERMARKET" at "//h2"</t>
+  </si>
+  <si>
+    <t>2.Click on "Show Invoice" at "(//a[contains(@href, '/invoice/')])[1]"</t>
+  </si>
+  <si>
+    <t>TC_LOGOUT_01</t>
+  </si>
+  <si>
+    <t>Verify Logout Functionality</t>
+  </si>
+  <si>
+    <t>2.Click on "Logout Button" at "//button[contains(@class, 'btn-logout')]"</t>
+  </si>
+  <si>
+    <t>3.Verify URL contains "login"</t>
   </si>
 </sst>
 </file>
@@ -1152,7 +1177,7 @@
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1830,10 +1855,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA48A5FA-3EC7-484B-B419-BAAFFEFDA622}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1875,87 +1900,159 @@
         <v>131</v>
       </c>
       <c r="B4" t="s">
-        <v>76</v>
+        <v>150</v>
       </c>
       <c r="C4" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>133</v>
-      </c>
-      <c r="B5" t="s">
-        <v>134</v>
-      </c>
       <c r="C5" t="s">
-        <v>138</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
-        <v>139</v>
+        <v>151</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
-        <v>140</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>133</v>
+      </c>
+      <c r="B9" t="s">
+        <v>134</v>
+      </c>
       <c r="C9" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C12" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>135</v>
-      </c>
-      <c r="B13" t="s">
-        <v>136</v>
-      </c>
       <c r="C13" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C16" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>135</v>
+      </c>
+      <c r="B17" t="s">
+        <v>136</v>
+      </c>
+      <c r="C17" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C18" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C19" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C20" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C17" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C21" t="s">
         <v>149</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50D50A06-F551-48F8-9461-013D23680FFD}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.6640625" customWidth="1"/>
+    <col min="2" max="2" width="26.5546875" customWidth="1"/>
+    <col min="3" max="3" width="60.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
27th commit with Signup admin database cleared
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/Nesto_TestCases.xlsx
+++ b/src/main/resources/testdata/Nesto_TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\EIT PROJECTS\Nesto_Automation_Framework\src\main\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C185C60D-8527-484E-9F78-A2783830AAF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE255357-794A-476A-9BEF-BEB7599764BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Auth_Tests" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="161">
   <si>
     <t>Test Steps</t>
   </si>
@@ -288,9 +288,6 @@
     <t>Verify Entry</t>
   </si>
   <si>
-    <t>1.dbexecute "{DB_QUERY}DELETE FROM customers WHERE email='auto@nesto.com'" at ""</t>
-  </si>
-  <si>
     <t>1.Open URL "http://localhost:8080/customers"</t>
   </si>
   <si>
@@ -499,6 +496,18 @@
   </si>
   <si>
     <t>3.Verify URL contains "login"</t>
+  </si>
+  <si>
+    <t>1.dbexecute "{DB_QUERY}DELETE FROM customers WHERE email='auto@nesto.com'"</t>
+  </si>
+  <si>
+    <t>TC_07</t>
+  </si>
+  <si>
+    <t>1.dbexecute "{DB_QUERY}DELETE FROM admins WHERE email LIKE 'nesto_admin_%'" at "//skip"</t>
+  </si>
+  <si>
+    <t>Delete Test SignUp  for Database Cleanup</t>
   </si>
 </sst>
 </file>
@@ -936,17 +945,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.44140625" customWidth="1"/>
-    <col min="2" max="2" width="32" customWidth="1"/>
-    <col min="3" max="3" width="74.109375" customWidth="1"/>
+    <col min="2" max="2" width="38" customWidth="1"/>
+    <col min="3" max="3" width="81.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -1053,116 +1062,127 @@
         <v>20</v>
       </c>
       <c r="B16" t="s">
+        <v>160</v>
+      </c>
+      <c r="C16" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" t="s">
         <v>21</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C17" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C17" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C18" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C19" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C21" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C22" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C24" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>28</v>
-      </c>
-      <c r="B24" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" t="s">
         <v>29</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C25" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C25" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C26" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C27" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>42</v>
-      </c>
-      <c r="B27" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>158</v>
+      </c>
+      <c r="B28" t="s">
         <v>34</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C28" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C28" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C30" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C31" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C32" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C33" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
     </row>
     <row r="34" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C34" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
     </row>
     <row r="35" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C35" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="36" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C36" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1415,7 +1435,7 @@
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
@@ -1549,7 +1569,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1605,7 +1625,7 @@
         <v>79</v>
       </c>
       <c r="C5" t="s">
-        <v>87</v>
+        <v>157</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -1641,54 +1661,54 @@
         <v>86</v>
       </c>
       <c r="C11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>90</v>
+      </c>
+      <c r="B13" t="s">
         <v>91</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>92</v>
-      </c>
-      <c r="C13" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>96</v>
+      </c>
+      <c r="B17" t="s">
         <v>97</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>98</v>
-      </c>
-      <c r="C17" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1724,13 +1744,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" t="s">
         <v>101</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>102</v>
-      </c>
-      <c r="C2" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1740,44 +1760,44 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B4" t="s">
         <v>76</v>
       </c>
       <c r="C4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B5" t="s">
         <v>106</v>
       </c>
-      <c r="B5" t="s">
-        <v>107</v>
-      </c>
       <c r="C5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -1787,65 +1807,65 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>111</v>
+      </c>
+      <c r="B11" t="s">
         <v>112</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>113</v>
-      </c>
-      <c r="C11" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>115</v>
+      </c>
+      <c r="B13" t="s">
+        <v>117</v>
+      </c>
+      <c r="C13" t="s">
         <v>116</v>
-      </c>
-      <c r="B13" t="s">
-        <v>118</v>
-      </c>
-      <c r="C13" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C17" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>123</v>
+      </c>
+      <c r="B18" t="s">
         <v>124</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>125</v>
-      </c>
-      <c r="C18" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C19" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -1881,13 +1901,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B2" t="s">
         <v>128</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>129</v>
-      </c>
-      <c r="C2" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1897,110 +1917,110 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B4" t="s">
+        <v>149</v>
+      </c>
+      <c r="C4" t="s">
         <v>131</v>
-      </c>
-      <c r="B4" t="s">
-        <v>150</v>
-      </c>
-      <c r="C4" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>132</v>
+      </c>
+      <c r="B9" t="s">
         <v>133</v>
       </c>
-      <c r="B9" t="s">
-        <v>134</v>
-      </c>
       <c r="C9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>134</v>
+      </c>
+      <c r="B17" t="s">
         <v>135</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>136</v>
-      </c>
-      <c r="C17" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C18" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C19" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C20" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -2012,8 +2032,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50D50A06-F551-48F8-9461-013D23680FFD}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2036,10 +2056,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B2" t="s">
         <v>154</v>
-      </c>
-      <c r="B2" t="s">
-        <v>155</v>
       </c>
       <c r="C2" t="s">
         <v>59</v>
@@ -2047,12 +2067,12 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
29th commit with error fixed
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/Nesto_TestCases.xlsx
+++ b/src/main/resources/testdata/Nesto_TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\EIT PROJECTS\Nesto_Automation_Framework\src\main\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE255357-794A-476A-9BEF-BEB7599764BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7448BD2-3A27-472A-A3CA-9184C7DAE010}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Auth_Tests" sheetId="1" r:id="rId1"/>
@@ -465,12 +465,6 @@
     <t>2.Verify text "faizal" at "//strong[text()='Customer:']/following-sibling::span"</t>
   </si>
   <si>
-    <t>3.Verify text "Dettol" at "//table/tbody/tr[1]/td[1]"</t>
-  </si>
-  <si>
-    <t>4.Verify text "Pears Soap" at "//table/tbody/tr[2]/td[1]"</t>
-  </si>
-  <si>
     <t>5.Click "Back" at "//a[text()='Back']"</t>
   </si>
   <si>
@@ -508,6 +502,12 @@
   </si>
   <si>
     <t>Delete Test SignUp  for Database Cleanup</t>
+  </si>
+  <si>
+    <t>3.Verify text "Pears Soap"" at "//table/tbody/tr[1]/td[1]"</t>
+  </si>
+  <si>
+    <t>4.Verify text "Dettol" at "//table/tbody/tr[2]/td[1]"</t>
   </si>
 </sst>
 </file>
@@ -947,7 +947,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -1062,10 +1062,10 @@
         <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C16" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -1137,7 +1137,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B28" t="s">
         <v>34</v>
@@ -1625,7 +1625,7 @@
         <v>79</v>
       </c>
       <c r="C5" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -1877,8 +1877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA48A5FA-3EC7-484B-B419-BAAFFEFDA622}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1920,7 +1920,7 @@
         <v>130</v>
       </c>
       <c r="B4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C4" t="s">
         <v>131</v>
@@ -1928,22 +1928,22 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -2010,17 +2010,17 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C19" t="s">
-        <v>146</v>
+        <v>159</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C20" t="s">
-        <v>147</v>
+        <v>160</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C21" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -2056,10 +2056,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C2" t="s">
         <v>59</v>
@@ -2067,12 +2067,12 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>

</xml_diff>